<commit_message>
significant development to optimizer, incomplete
</commit_message>
<xml_diff>
--- a/may-pipeline/Attribution Table.xlsx
+++ b/may-pipeline/Attribution Table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Revenue Contributions</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>youtube_media_cost</t>
+  </si>
+  <si>
+    <t>googlesearch_media_cost</t>
+  </si>
+  <si>
+    <t>dv360_media_cost</t>
   </si>
 </sst>
 </file>
@@ -389,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -411,13 +417,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>193.3129926225687</v>
+        <v>167.5429929727877</v>
       </c>
       <c r="C2">
         <v>947.5823100035</v>
       </c>
       <c r="D2">
-        <v>0.204006544425523</v>
+        <v>0.176811018107935</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -425,13 +431,13 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>35664.11793319909</v>
+        <v>31331.46756994809</v>
       </c>
       <c r="C3">
         <v>3079426.160085</v>
       </c>
       <c r="D3">
-        <v>0.01158141682222206</v>
+        <v>0.01017445002450822</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -439,13 +445,41 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>23647.56645148726</v>
+        <v>23995.74187856295</v>
       </c>
       <c r="C4">
         <v>229054.302767</v>
       </c>
       <c r="D4">
-        <v>0.1032400010208155</v>
+        <v>0.1047600572820151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>44668.42512772494</v>
+      </c>
+      <c r="C5">
+        <v>1494447.761988</v>
+      </c>
+      <c r="D5">
+        <v>0.02988958614940441</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>477.8417833700823</v>
+      </c>
+      <c r="C6">
+        <v>271129.18</v>
+      </c>
+      <c r="D6">
+        <v>0.001762413707628527</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimizer complete, attribution table file name changed, export for optimizer created, code needs to be cleaned up further, forecast needs to be tweaked, final minor changes in untitled.md
</commit_message>
<xml_diff>
--- a/may-pipeline/Attribution Table.xlsx
+++ b/may-pipeline/Attribution Table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Revenue Contributions</t>
   </si>
@@ -28,16 +28,49 @@
     <t>amazon_media_cost</t>
   </si>
   <si>
+    <t>bingsearch_media_cost</t>
+  </si>
+  <si>
+    <t>ctv_media_cost</t>
+  </si>
+  <si>
+    <t>criteo_media_cost</t>
+  </si>
+  <si>
+    <t>dv360_media_cost</t>
+  </si>
+  <si>
     <t>facebook_media_cost</t>
   </si>
   <si>
+    <t>googlesearch_media_cost</t>
+  </si>
+  <si>
+    <t>influential_media_cost</t>
+  </si>
+  <si>
+    <t>lineartv_media_cost</t>
+  </si>
+  <si>
+    <t>pinterest_media_cost</t>
+  </si>
+  <si>
+    <t>radio_media_cost</t>
+  </si>
+  <si>
+    <t>snapchat_media_cost</t>
+  </si>
+  <si>
+    <t>thetradedesk_media_cost</t>
+  </si>
+  <si>
+    <t>tinder_media_cost</t>
+  </si>
+  <si>
+    <t>twitch_media_cost</t>
+  </si>
+  <si>
     <t>youtube_media_cost</t>
-  </si>
-  <si>
-    <t>googlesearch_media_cost</t>
-  </si>
-  <si>
-    <t>dv360_media_cost</t>
   </si>
 </sst>
 </file>
@@ -395,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -417,13 +450,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>167.5429929727877</v>
+        <v>325.4689352158736</v>
       </c>
       <c r="C2">
         <v>947.5823100035</v>
       </c>
       <c r="D2">
-        <v>0.176811018107935</v>
+        <v>0.3434729962557779</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -431,13 +464,13 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>31331.46756994809</v>
+        <v>18604.99254492222</v>
       </c>
       <c r="C3">
-        <v>3079426.160085</v>
+        <v>71190.62</v>
       </c>
       <c r="D3">
-        <v>0.01017445002450822</v>
+        <v>0.2613405044782897</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -445,13 +478,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>23995.74187856295</v>
+        <v>1370.421463794661</v>
       </c>
       <c r="C4">
-        <v>229054.302767</v>
+        <v>932751.4633993</v>
       </c>
       <c r="D4">
-        <v>0.1047600572820151</v>
+        <v>0.001469224672990944</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -459,13 +492,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>44668.42512772494</v>
+        <v>34.99542947131734</v>
       </c>
       <c r="C5">
-        <v>1494447.761988</v>
+        <v>145.4036846402</v>
       </c>
       <c r="D5">
-        <v>0.02988958614940441</v>
+        <v>0.240677734941265</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -473,13 +506,164 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>477.8417833700823</v>
+        <v>618.4626357864217</v>
       </c>
       <c r="C6">
         <v>271129.18</v>
       </c>
       <c r="D6">
-        <v>0.001762413707628527</v>
+        <v>0.002281062612981833</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>31233.80555115086</v>
+      </c>
+      <c r="C7">
+        <v>3079426.160085</v>
+      </c>
+      <c r="D7">
+        <v>0.01014273566809237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>32679.13737021944</v>
+      </c>
+      <c r="C8">
+        <v>1494447.761988</v>
+      </c>
+      <c r="D8">
+        <v>0.02186703222516643</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>1282.53220170682</v>
+      </c>
+      <c r="C9">
+        <v>109551.439979</v>
+      </c>
+      <c r="D9">
+        <v>0.01170712317385029</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>1445.577637401062</v>
+      </c>
+      <c r="C10">
+        <v>1467680</v>
+      </c>
+      <c r="D10">
+        <v>0.0009849406119869875</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>3661.441939006166</v>
+      </c>
+      <c r="C11">
+        <v>21588.25</v>
+      </c>
+      <c r="D11">
+        <v>0.1696034620224504</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>727.1401467448559</v>
+      </c>
+      <c r="C13">
+        <v>957.659705</v>
+      </c>
+      <c r="D13">
+        <v>0.7592886522722138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>1639.986963078731</v>
+      </c>
+      <c r="C14">
+        <v>133960.5438629989</v>
+      </c>
+      <c r="D14">
+        <v>0.0122423134139851</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>176.9075242613488</v>
+      </c>
+      <c r="C15">
+        <v>56425.47</v>
+      </c>
+      <c r="D15">
+        <v>0.003135242369471603</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>50.96558290840737</v>
+      </c>
+      <c r="C16">
+        <v>12709.62</v>
+      </c>
+      <c r="D16">
+        <v>0.004010000527821239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>29554.89816805543</v>
+      </c>
+      <c r="C17">
+        <v>229054.302767</v>
+      </c>
+      <c r="D17">
+        <v>0.1290300937857493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>